<commit_message>
Fin de la version 0.1
</commit_message>
<xml_diff>
--- a/Documentation/Sénar.xlsx
+++ b/Documentation/Sénar.xlsx
@@ -77,9 +77,6 @@
     <t>Savoir jouer a la BN</t>
   </si>
   <si>
-    <t>L'application me demande de saisir mes première coordonée</t>
-  </si>
-  <si>
     <t>Avoir apris a jouer</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
     <t>J'entre mes premières
 coordonées et j'observe ce qui
 se passe</t>
+  </si>
+  <si>
+    <t>L'application me demande de saisir mes premières coordonées</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C11" sqref="C11:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -718,7 +718,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -759,10 +759,10 @@
     </row>
     <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>14</v>
@@ -770,13 +770,13 @@
     </row>
     <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -789,10 +789,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -807,11 +807,11 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="12"/>
     </row>
@@ -924,7 +924,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -941,7 +941,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>13</v>
@@ -952,13 +952,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -973,13 +973,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="11"/>
     </row>
@@ -1038,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="11"/>
     </row>
@@ -1047,7 +1047,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="11"/>
     </row>
@@ -1056,7 +1056,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>37</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1105,22 +1105,22 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
       <c r="B13" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>29</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1154,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1170,7 +1170,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1178,7 +1178,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1186,7 +1186,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>14</v>
@@ -1214,13 +1214,13 @@
     </row>
     <row r="9" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>